<commit_message>
changes made to rid of the 'PDB molecule' column in the metadata input file
</commit_message>
<xml_diff>
--- a/test/data/pdb_metafile_sample1a.xlsx
+++ b/test/data/pdb_metafile_sample1a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qzhang/qzwk_dir/qzModules/ProteinStructureUtils/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D092D77-2639-6F4D-BE40-2FD5DB5DAC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716170DA-AE9E-0842-A567-0DCACFD34D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="980" windowWidth="25040" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Narrative ID</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Feature ID</t>
   </si>
   <si>
-    <t>PDB molecule</t>
-  </si>
-  <si>
     <t>PDB filename</t>
   </si>
   <si>
@@ -43,16 +40,10 @@
     <t>JCVISYN3_0001</t>
   </si>
   <si>
-    <t>chain1</t>
-  </si>
-  <si>
     <t>JCVISYN3_0001.pdb</t>
   </si>
   <si>
     <t>JCVISYN3_0002</t>
-  </si>
-  <si>
-    <t>chain2</t>
   </si>
   <si>
     <t>JCVISYN3_0003</t>
@@ -908,20 +899,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -934,94 +926,85 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50569</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>50569</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>50569</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50569</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>50569</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>50569</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>50569</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with the merged ProteinStructure, re-wrote the code and redesign the html report using mol*
</commit_message>
<xml_diff>
--- a/test/data/pdb_metafile_sample1a.xlsx
+++ b/test/data/pdb_metafile_sample1a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qzhang/qzwk_dir/qzModules/ProteinStructureUtils/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716170DA-AE9E-0842-A567-0DCACFD34D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92362585-AC9F-5646-9F0F-04A66D17AB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="980" windowWidth="25040" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Narrative ID</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>JCVI_Syn1</t>
+  </si>
+  <si>
+    <t>Is model</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -899,21 +908,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -926,8 +935,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50569</v>
       </c>
@@ -940,8 +952,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>50569</v>
       </c>
@@ -954,8 +969,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>50569</v>
       </c>
@@ -968,8 +986,11 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50569</v>
       </c>
@@ -982,8 +1003,11 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>50569</v>
       </c>
@@ -991,7 +1015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>50569</v>
       </c>
@@ -999,7 +1023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>50569</v>
       </c>

</xml_diff>

<commit_message>
consolidate input metafile file contents to cover uploader and rcsb importer, updated test files and ran the first batch of tests
</commit_message>
<xml_diff>
--- a/test/data/pdb_metafile_sample1a.xlsx
+++ b/test/data/pdb_metafile_sample1a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qzhang/qzwk_dir/qzModules/ProteinStructureUtils/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92362585-AC9F-5646-9F0F-04A66D17AB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A57FFC9-72A4-3544-8728-872348E61E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="980" windowWidth="25040" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="900" windowWidth="25040" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pdb_metafile_sample" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Narrative ID</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Feature ID</t>
   </si>
   <si>
-    <t>PDB filename</t>
-  </si>
-  <si>
     <t>JCVI_Syn3.kbase</t>
   </si>
   <si>
@@ -61,13 +58,25 @@
     <t>JCVI_Syn1</t>
   </si>
   <si>
-    <t>Is model</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>pdb</t>
+  </si>
+  <si>
+    <t>PDB or RCSB ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Is model</t>
+  </si>
+  <si>
+    <t>From RCSB</t>
+  </si>
+  <si>
+    <t>File Extension</t>
   </si>
 </sst>
 </file>
@@ -908,21 +917,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="3" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -933,102 +942,132 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50569</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>50569</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>50569</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50569</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>50569</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>50569</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>50569</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>